<commit_message>
add to dynamic grid
</commit_message>
<xml_diff>
--- a/assignment11/hw11.xlsx
+++ b/assignment11/hw11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bth/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q8517\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25FE39D5-7BF1-8047-944E-BB6E629EC5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0B1585-8AA0-4533-B961-037754C8B07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="2800" windowWidth="28040" windowHeight="16380" xr2:uid="{ACE5AE64-2FA3-3E4F-A211-9D0322AE665D}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{ACE5AE64-2FA3-3E4F-A211-9D0322AE665D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Name:</t>
-  </si>
-  <si>
-    <t>Email:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Homework for Module 11</t>
   </si>
@@ -93,6 +87,78 @@
   </si>
   <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>Name: Leo Liang</t>
+  </si>
+  <si>
+    <t>Email: liang.jiahao@northeastern.edu</t>
+  </si>
+  <si>
+    <t>4N</t>
+  </si>
+  <si>
+    <t>5N</t>
+  </si>
+  <si>
+    <t>6N</t>
+  </si>
+  <si>
+    <t>7N</t>
+  </si>
+  <si>
+    <t>8N</t>
+  </si>
+  <si>
+    <t>9N</t>
+  </si>
+  <si>
+    <t>10N</t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>4D</t>
+  </si>
+  <si>
+    <t>5D</t>
+  </si>
+  <si>
+    <t>1Q</t>
+  </si>
+  <si>
+    <t>1D 1N</t>
+  </si>
+  <si>
+    <t>2D 1N</t>
+  </si>
+  <si>
+    <t>1Q 1N</t>
+  </si>
+  <si>
+    <t>1Q 1D</t>
+  </si>
+  <si>
+    <t>3D 1N</t>
+  </si>
+  <si>
+    <t>1Q 2D</t>
+  </si>
+  <si>
+    <t>4D 1N</t>
+  </si>
+  <si>
+    <t>2Q</t>
+  </si>
+  <si>
+    <t>1Q 1D 1N</t>
   </si>
 </sst>
 </file>
@@ -551,72 +617,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A045F9A-EC6B-5643-86DC-3E05D9A16DB6}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="75.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="18.45" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1" ht="47.6" x14ac:dyDescent="0.45">
+      <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="7"/>
+    </row>
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="31.75" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:13" s="1" customFormat="1" ht="63.45" x14ac:dyDescent="0.45">
+      <c r="A12" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-    </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+    <row r="13" spans="1:13" ht="16.3" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:13" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-    </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="C14" s="3" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="D14" s="3">
         <v>5</v>
@@ -649,65 +715,119 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15" s="5">
         <v>5</v>
       </c>
       <c r="D15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="G15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-    </row>
-    <row r="16" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C16" s="5">
         <v>10</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B17" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" s="5">
         <v>25</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>